<commit_message>
updated conditions, fixed generator
</commit_message>
<xml_diff>
--- a/file_generators/conditions/10m-for-2d-0700to1700_28C-20C_55rh_heliospectra_s7.xlsx
+++ b/file_generators/conditions/10m-for-2d-0700to1700_28C-20C_55rh_heliospectra_s7.xlsx
@@ -418,10 +418,10 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>43854</v>
+        <v>43875</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>43854</v>
+        <v>43875</v>
       </c>
       <c r="C2" t="n">
         <v>55</v>
@@ -453,10 +453,10 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>43854.00694444445</v>
+        <v>43875.00694444445</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>43854.00694444445</v>
+        <v>43875.00694444445</v>
       </c>
       <c r="C3" t="n">
         <v>55</v>
@@ -488,10 +488,10 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>43854.01388888889</v>
+        <v>43875.01388888889</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>43854.01388888889</v>
+        <v>43875.01388888889</v>
       </c>
       <c r="C4" t="n">
         <v>55</v>
@@ -523,10 +523,10 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>43854.02083333334</v>
+        <v>43875.02083333334</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>43854.02083333334</v>
+        <v>43875.02083333334</v>
       </c>
       <c r="C5" t="n">
         <v>55</v>
@@ -558,10 +558,10 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>43854.02777777778</v>
+        <v>43875.02777777778</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>43854.02777777778</v>
+        <v>43875.02777777778</v>
       </c>
       <c r="C6" t="n">
         <v>55</v>
@@ -593,10 +593,10 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>43854.03472222222</v>
+        <v>43875.03472222222</v>
       </c>
       <c r="B7" s="1" t="n">
-        <v>43854.03472222222</v>
+        <v>43875.03472222222</v>
       </c>
       <c r="C7" t="n">
         <v>55</v>
@@ -628,10 +628,10 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>43854.04166666666</v>
+        <v>43875.04166666666</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>43854.04166666666</v>
+        <v>43875.04166666666</v>
       </c>
       <c r="C8" t="n">
         <v>55</v>
@@ -663,10 +663,10 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>43854.04861111111</v>
+        <v>43875.04861111111</v>
       </c>
       <c r="B9" s="1" t="n">
-        <v>43854.04861111111</v>
+        <v>43875.04861111111</v>
       </c>
       <c r="C9" t="n">
         <v>55</v>
@@ -698,10 +698,10 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>43854.05555555555</v>
+        <v>43875.05555555555</v>
       </c>
       <c r="B10" s="1" t="n">
-        <v>43854.05555555555</v>
+        <v>43875.05555555555</v>
       </c>
       <c r="C10" t="n">
         <v>55</v>
@@ -733,10 +733,10 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>43854.0625</v>
+        <v>43875.0625</v>
       </c>
       <c r="B11" s="1" t="n">
-        <v>43854.0625</v>
+        <v>43875.0625</v>
       </c>
       <c r="C11" t="n">
         <v>55</v>
@@ -768,10 +768,10 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>43854.06944444445</v>
+        <v>43875.06944444445</v>
       </c>
       <c r="B12" s="1" t="n">
-        <v>43854.06944444445</v>
+        <v>43875.06944444445</v>
       </c>
       <c r="C12" t="n">
         <v>55</v>
@@ -803,10 +803,10 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>43854.07638888889</v>
+        <v>43875.07638888889</v>
       </c>
       <c r="B13" s="1" t="n">
-        <v>43854.07638888889</v>
+        <v>43875.07638888889</v>
       </c>
       <c r="C13" t="n">
         <v>55</v>
@@ -838,10 +838,10 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>43854.08333333334</v>
+        <v>43875.08333333334</v>
       </c>
       <c r="B14" s="1" t="n">
-        <v>43854.08333333334</v>
+        <v>43875.08333333334</v>
       </c>
       <c r="C14" t="n">
         <v>55</v>
@@ -873,10 +873,10 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>43854.09027777778</v>
+        <v>43875.09027777778</v>
       </c>
       <c r="B15" s="1" t="n">
-        <v>43854.09027777778</v>
+        <v>43875.09027777778</v>
       </c>
       <c r="C15" t="n">
         <v>55</v>
@@ -908,10 +908,10 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>43854.09722222222</v>
+        <v>43875.09722222222</v>
       </c>
       <c r="B16" s="1" t="n">
-        <v>43854.09722222222</v>
+        <v>43875.09722222222</v>
       </c>
       <c r="C16" t="n">
         <v>55</v>
@@ -943,10 +943,10 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>43854.10416666666</v>
+        <v>43875.10416666666</v>
       </c>
       <c r="B17" s="1" t="n">
-        <v>43854.10416666666</v>
+        <v>43875.10416666666</v>
       </c>
       <c r="C17" t="n">
         <v>55</v>
@@ -978,10 +978,10 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>43854.11111111111</v>
+        <v>43875.11111111111</v>
       </c>
       <c r="B18" s="1" t="n">
-        <v>43854.11111111111</v>
+        <v>43875.11111111111</v>
       </c>
       <c r="C18" t="n">
         <v>55</v>
@@ -1013,10 +1013,10 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>43854.11805555555</v>
+        <v>43875.11805555555</v>
       </c>
       <c r="B19" s="1" t="n">
-        <v>43854.11805555555</v>
+        <v>43875.11805555555</v>
       </c>
       <c r="C19" t="n">
         <v>55</v>
@@ -1048,10 +1048,10 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>43854.125</v>
+        <v>43875.125</v>
       </c>
       <c r="B20" s="1" t="n">
-        <v>43854.125</v>
+        <v>43875.125</v>
       </c>
       <c r="C20" t="n">
         <v>55</v>
@@ -1083,10 +1083,10 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>43854.13194444445</v>
+        <v>43875.13194444445</v>
       </c>
       <c r="B21" s="1" t="n">
-        <v>43854.13194444445</v>
+        <v>43875.13194444445</v>
       </c>
       <c r="C21" t="n">
         <v>55</v>
@@ -1118,10 +1118,10 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>43854.13888888889</v>
+        <v>43875.13888888889</v>
       </c>
       <c r="B22" s="1" t="n">
-        <v>43854.13888888889</v>
+        <v>43875.13888888889</v>
       </c>
       <c r="C22" t="n">
         <v>55</v>
@@ -1153,10 +1153,10 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>43854.14583333334</v>
+        <v>43875.14583333334</v>
       </c>
       <c r="B23" s="1" t="n">
-        <v>43854.14583333334</v>
+        <v>43875.14583333334</v>
       </c>
       <c r="C23" t="n">
         <v>55</v>
@@ -1188,10 +1188,10 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>43854.15277777778</v>
+        <v>43875.15277777778</v>
       </c>
       <c r="B24" s="1" t="n">
-        <v>43854.15277777778</v>
+        <v>43875.15277777778</v>
       </c>
       <c r="C24" t="n">
         <v>55</v>
@@ -1223,10 +1223,10 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>43854.15972222222</v>
+        <v>43875.15972222222</v>
       </c>
       <c r="B25" s="1" t="n">
-        <v>43854.15972222222</v>
+        <v>43875.15972222222</v>
       </c>
       <c r="C25" t="n">
         <v>55</v>
@@ -1258,10 +1258,10 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>43854.16666666666</v>
+        <v>43875.16666666666</v>
       </c>
       <c r="B26" s="1" t="n">
-        <v>43854.16666666666</v>
+        <v>43875.16666666666</v>
       </c>
       <c r="C26" t="n">
         <v>55</v>
@@ -1293,10 +1293,10 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>43854.17361111111</v>
+        <v>43875.17361111111</v>
       </c>
       <c r="B27" s="1" t="n">
-        <v>43854.17361111111</v>
+        <v>43875.17361111111</v>
       </c>
       <c r="C27" t="n">
         <v>55</v>
@@ -1328,10 +1328,10 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>43854.18055555555</v>
+        <v>43875.18055555555</v>
       </c>
       <c r="B28" s="1" t="n">
-        <v>43854.18055555555</v>
+        <v>43875.18055555555</v>
       </c>
       <c r="C28" t="n">
         <v>55</v>
@@ -1363,10 +1363,10 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>43854.1875</v>
+        <v>43875.1875</v>
       </c>
       <c r="B29" s="1" t="n">
-        <v>43854.1875</v>
+        <v>43875.1875</v>
       </c>
       <c r="C29" t="n">
         <v>55</v>
@@ -1398,10 +1398,10 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>43854.19444444445</v>
+        <v>43875.19444444445</v>
       </c>
       <c r="B30" s="1" t="n">
-        <v>43854.19444444445</v>
+        <v>43875.19444444445</v>
       </c>
       <c r="C30" t="n">
         <v>55</v>
@@ -1433,10 +1433,10 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>43854.20138888889</v>
+        <v>43875.20138888889</v>
       </c>
       <c r="B31" s="1" t="n">
-        <v>43854.20138888889</v>
+        <v>43875.20138888889</v>
       </c>
       <c r="C31" t="n">
         <v>55</v>
@@ -1468,10 +1468,10 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>43854.20833333334</v>
+        <v>43875.20833333334</v>
       </c>
       <c r="B32" s="1" t="n">
-        <v>43854.20833333334</v>
+        <v>43875.20833333334</v>
       </c>
       <c r="C32" t="n">
         <v>55</v>
@@ -1503,10 +1503,10 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>43854.21527777778</v>
+        <v>43875.21527777778</v>
       </c>
       <c r="B33" s="1" t="n">
-        <v>43854.21527777778</v>
+        <v>43875.21527777778</v>
       </c>
       <c r="C33" t="n">
         <v>55</v>
@@ -1538,10 +1538,10 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>43854.22222222222</v>
+        <v>43875.22222222222</v>
       </c>
       <c r="B34" s="1" t="n">
-        <v>43854.22222222222</v>
+        <v>43875.22222222222</v>
       </c>
       <c r="C34" t="n">
         <v>55</v>
@@ -1573,10 +1573,10 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>43854.22916666666</v>
+        <v>43875.22916666666</v>
       </c>
       <c r="B35" s="1" t="n">
-        <v>43854.22916666666</v>
+        <v>43875.22916666666</v>
       </c>
       <c r="C35" t="n">
         <v>55</v>
@@ -1608,10 +1608,10 @@
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>43854.23611111111</v>
+        <v>43875.23611111111</v>
       </c>
       <c r="B36" s="1" t="n">
-        <v>43854.23611111111</v>
+        <v>43875.23611111111</v>
       </c>
       <c r="C36" t="n">
         <v>55</v>
@@ -1643,10 +1643,10 @@
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>43854.24305555555</v>
+        <v>43875.24305555555</v>
       </c>
       <c r="B37" s="1" t="n">
-        <v>43854.24305555555</v>
+        <v>43875.24305555555</v>
       </c>
       <c r="C37" t="n">
         <v>55</v>
@@ -1678,10 +1678,10 @@
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>43854.25</v>
+        <v>43875.25</v>
       </c>
       <c r="B38" s="1" t="n">
-        <v>43854.25</v>
+        <v>43875.25</v>
       </c>
       <c r="C38" t="n">
         <v>55</v>
@@ -1713,10 +1713,10 @@
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>43854.25694444445</v>
+        <v>43875.25694444445</v>
       </c>
       <c r="B39" s="1" t="n">
-        <v>43854.25694444445</v>
+        <v>43875.25694444445</v>
       </c>
       <c r="C39" t="n">
         <v>55</v>
@@ -1748,10 +1748,10 @@
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>43854.26388888889</v>
+        <v>43875.26388888889</v>
       </c>
       <c r="B40" s="1" t="n">
-        <v>43854.26388888889</v>
+        <v>43875.26388888889</v>
       </c>
       <c r="C40" t="n">
         <v>55</v>
@@ -1783,10 +1783,10 @@
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>43854.27083333334</v>
+        <v>43875.27083333334</v>
       </c>
       <c r="B41" s="1" t="n">
-        <v>43854.27083333334</v>
+        <v>43875.27083333334</v>
       </c>
       <c r="C41" t="n">
         <v>55</v>
@@ -1818,10 +1818,10 @@
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>43854.27777777778</v>
+        <v>43875.27777777778</v>
       </c>
       <c r="B42" s="1" t="n">
-        <v>43854.27777777778</v>
+        <v>43875.27777777778</v>
       </c>
       <c r="C42" t="n">
         <v>55</v>
@@ -1853,10 +1853,10 @@
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>43854.28472222222</v>
+        <v>43875.28472222222</v>
       </c>
       <c r="B43" s="1" t="n">
-        <v>43854.28472222222</v>
+        <v>43875.28472222222</v>
       </c>
       <c r="C43" t="n">
         <v>55</v>
@@ -1888,10 +1888,10 @@
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>43854.29166666666</v>
+        <v>43875.29166666666</v>
       </c>
       <c r="B44" s="1" t="n">
-        <v>43854.29166666666</v>
+        <v>43875.29166666666</v>
       </c>
       <c r="C44" t="n">
         <v>55</v>
@@ -1923,10 +1923,10 @@
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>43854.29861111111</v>
+        <v>43875.29861111111</v>
       </c>
       <c r="B45" s="1" t="n">
-        <v>43854.29861111111</v>
+        <v>43875.29861111111</v>
       </c>
       <c r="C45" t="n">
         <v>55</v>
@@ -1958,10 +1958,10 @@
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>43854.30555555555</v>
+        <v>43875.30555555555</v>
       </c>
       <c r="B46" s="1" t="n">
-        <v>43854.30555555555</v>
+        <v>43875.30555555555</v>
       </c>
       <c r="C46" t="n">
         <v>55</v>
@@ -1993,10 +1993,10 @@
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>43854.3125</v>
+        <v>43875.3125</v>
       </c>
       <c r="B47" s="1" t="n">
-        <v>43854.3125</v>
+        <v>43875.3125</v>
       </c>
       <c r="C47" t="n">
         <v>55</v>
@@ -2028,10 +2028,10 @@
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>43854.31944444445</v>
+        <v>43875.31944444445</v>
       </c>
       <c r="B48" s="1" t="n">
-        <v>43854.31944444445</v>
+        <v>43875.31944444445</v>
       </c>
       <c r="C48" t="n">
         <v>55</v>
@@ -2063,10 +2063,10 @@
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>43854.32638888889</v>
+        <v>43875.32638888889</v>
       </c>
       <c r="B49" s="1" t="n">
-        <v>43854.32638888889</v>
+        <v>43875.32638888889</v>
       </c>
       <c r="C49" t="n">
         <v>55</v>
@@ -2098,10 +2098,10 @@
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>43854.33333333334</v>
+        <v>43875.33333333334</v>
       </c>
       <c r="B50" s="1" t="n">
-        <v>43854.33333333334</v>
+        <v>43875.33333333334</v>
       </c>
       <c r="C50" t="n">
         <v>55</v>
@@ -2133,10 +2133,10 @@
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>43854.34027777778</v>
+        <v>43875.34027777778</v>
       </c>
       <c r="B51" s="1" t="n">
-        <v>43854.34027777778</v>
+        <v>43875.34027777778</v>
       </c>
       <c r="C51" t="n">
         <v>55</v>
@@ -2168,10 +2168,10 @@
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>43854.34722222222</v>
+        <v>43875.34722222222</v>
       </c>
       <c r="B52" s="1" t="n">
-        <v>43854.34722222222</v>
+        <v>43875.34722222222</v>
       </c>
       <c r="C52" t="n">
         <v>55</v>
@@ -2203,10 +2203,10 @@
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>43854.35416666666</v>
+        <v>43875.35416666666</v>
       </c>
       <c r="B53" s="1" t="n">
-        <v>43854.35416666666</v>
+        <v>43875.35416666666</v>
       </c>
       <c r="C53" t="n">
         <v>55</v>
@@ -2238,10 +2238,10 @@
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>43854.36111111111</v>
+        <v>43875.36111111111</v>
       </c>
       <c r="B54" s="1" t="n">
-        <v>43854.36111111111</v>
+        <v>43875.36111111111</v>
       </c>
       <c r="C54" t="n">
         <v>55</v>
@@ -2273,10 +2273,10 @@
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>43854.36805555555</v>
+        <v>43875.36805555555</v>
       </c>
       <c r="B55" s="1" t="n">
-        <v>43854.36805555555</v>
+        <v>43875.36805555555</v>
       </c>
       <c r="C55" t="n">
         <v>55</v>
@@ -2308,10 +2308,10 @@
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>43854.375</v>
+        <v>43875.375</v>
       </c>
       <c r="B56" s="1" t="n">
-        <v>43854.375</v>
+        <v>43875.375</v>
       </c>
       <c r="C56" t="n">
         <v>55</v>
@@ -2343,10 +2343,10 @@
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>43854.38194444445</v>
+        <v>43875.38194444445</v>
       </c>
       <c r="B57" s="1" t="n">
-        <v>43854.38194444445</v>
+        <v>43875.38194444445</v>
       </c>
       <c r="C57" t="n">
         <v>55</v>
@@ -2378,10 +2378,10 @@
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>43854.38888888889</v>
+        <v>43875.38888888889</v>
       </c>
       <c r="B58" s="1" t="n">
-        <v>43854.38888888889</v>
+        <v>43875.38888888889</v>
       </c>
       <c r="C58" t="n">
         <v>55</v>
@@ -2413,10 +2413,10 @@
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>43854.39583333334</v>
+        <v>43875.39583333334</v>
       </c>
       <c r="B59" s="1" t="n">
-        <v>43854.39583333334</v>
+        <v>43875.39583333334</v>
       </c>
       <c r="C59" t="n">
         <v>55</v>
@@ -2448,10 +2448,10 @@
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>43854.40277777778</v>
+        <v>43875.40277777778</v>
       </c>
       <c r="B60" s="1" t="n">
-        <v>43854.40277777778</v>
+        <v>43875.40277777778</v>
       </c>
       <c r="C60" t="n">
         <v>55</v>
@@ -2483,10 +2483,10 @@
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
-        <v>43854.40972222222</v>
+        <v>43875.40972222222</v>
       </c>
       <c r="B61" s="1" t="n">
-        <v>43854.40972222222</v>
+        <v>43875.40972222222</v>
       </c>
       <c r="C61" t="n">
         <v>55</v>
@@ -2518,10 +2518,10 @@
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>43854.41666666666</v>
+        <v>43875.41666666666</v>
       </c>
       <c r="B62" s="1" t="n">
-        <v>43854.41666666666</v>
+        <v>43875.41666666666</v>
       </c>
       <c r="C62" t="n">
         <v>55</v>
@@ -2553,10 +2553,10 @@
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>43854.42361111111</v>
+        <v>43875.42361111111</v>
       </c>
       <c r="B63" s="1" t="n">
-        <v>43854.42361111111</v>
+        <v>43875.42361111111</v>
       </c>
       <c r="C63" t="n">
         <v>55</v>
@@ -2588,10 +2588,10 @@
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>43854.43055555555</v>
+        <v>43875.43055555555</v>
       </c>
       <c r="B64" s="1" t="n">
-        <v>43854.43055555555</v>
+        <v>43875.43055555555</v>
       </c>
       <c r="C64" t="n">
         <v>55</v>
@@ -2623,10 +2623,10 @@
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>43854.4375</v>
+        <v>43875.4375</v>
       </c>
       <c r="B65" s="1" t="n">
-        <v>43854.4375</v>
+        <v>43875.4375</v>
       </c>
       <c r="C65" t="n">
         <v>55</v>
@@ -2658,10 +2658,10 @@
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>43854.44444444445</v>
+        <v>43875.44444444445</v>
       </c>
       <c r="B66" s="1" t="n">
-        <v>43854.44444444445</v>
+        <v>43875.44444444445</v>
       </c>
       <c r="C66" t="n">
         <v>55</v>
@@ -2693,10 +2693,10 @@
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>43854.45138888889</v>
+        <v>43875.45138888889</v>
       </c>
       <c r="B67" s="1" t="n">
-        <v>43854.45138888889</v>
+        <v>43875.45138888889</v>
       </c>
       <c r="C67" t="n">
         <v>55</v>
@@ -2728,10 +2728,10 @@
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>43854.45833333334</v>
+        <v>43875.45833333334</v>
       </c>
       <c r="B68" s="1" t="n">
-        <v>43854.45833333334</v>
+        <v>43875.45833333334</v>
       </c>
       <c r="C68" t="n">
         <v>55</v>
@@ -2763,10 +2763,10 @@
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>43854.46527777778</v>
+        <v>43875.46527777778</v>
       </c>
       <c r="B69" s="1" t="n">
-        <v>43854.46527777778</v>
+        <v>43875.46527777778</v>
       </c>
       <c r="C69" t="n">
         <v>55</v>
@@ -2798,10 +2798,10 @@
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>43854.47222222222</v>
+        <v>43875.47222222222</v>
       </c>
       <c r="B70" s="1" t="n">
-        <v>43854.47222222222</v>
+        <v>43875.47222222222</v>
       </c>
       <c r="C70" t="n">
         <v>55</v>
@@ -2833,10 +2833,10 @@
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
-        <v>43854.47916666666</v>
+        <v>43875.47916666666</v>
       </c>
       <c r="B71" s="1" t="n">
-        <v>43854.47916666666</v>
+        <v>43875.47916666666</v>
       </c>
       <c r="C71" t="n">
         <v>55</v>
@@ -2868,10 +2868,10 @@
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
-        <v>43854.48611111111</v>
+        <v>43875.48611111111</v>
       </c>
       <c r="B72" s="1" t="n">
-        <v>43854.48611111111</v>
+        <v>43875.48611111111</v>
       </c>
       <c r="C72" t="n">
         <v>55</v>
@@ -2903,10 +2903,10 @@
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
-        <v>43854.49305555555</v>
+        <v>43875.49305555555</v>
       </c>
       <c r="B73" s="1" t="n">
-        <v>43854.49305555555</v>
+        <v>43875.49305555555</v>
       </c>
       <c r="C73" t="n">
         <v>55</v>
@@ -2938,10 +2938,10 @@
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
-        <v>43854.5</v>
+        <v>43875.5</v>
       </c>
       <c r="B74" s="1" t="n">
-        <v>43854.5</v>
+        <v>43875.5</v>
       </c>
       <c r="C74" t="n">
         <v>55</v>
@@ -2973,10 +2973,10 @@
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
-        <v>43854.50694444445</v>
+        <v>43875.50694444445</v>
       </c>
       <c r="B75" s="1" t="n">
-        <v>43854.50694444445</v>
+        <v>43875.50694444445</v>
       </c>
       <c r="C75" t="n">
         <v>55</v>
@@ -3008,10 +3008,10 @@
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
-        <v>43854.51388888889</v>
+        <v>43875.51388888889</v>
       </c>
       <c r="B76" s="1" t="n">
-        <v>43854.51388888889</v>
+        <v>43875.51388888889</v>
       </c>
       <c r="C76" t="n">
         <v>55</v>
@@ -3043,10 +3043,10 @@
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
-        <v>43854.52083333334</v>
+        <v>43875.52083333334</v>
       </c>
       <c r="B77" s="1" t="n">
-        <v>43854.52083333334</v>
+        <v>43875.52083333334</v>
       </c>
       <c r="C77" t="n">
         <v>55</v>
@@ -3078,10 +3078,10 @@
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
-        <v>43854.52777777778</v>
+        <v>43875.52777777778</v>
       </c>
       <c r="B78" s="1" t="n">
-        <v>43854.52777777778</v>
+        <v>43875.52777777778</v>
       </c>
       <c r="C78" t="n">
         <v>55</v>
@@ -3113,10 +3113,10 @@
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
-        <v>43854.53472222222</v>
+        <v>43875.53472222222</v>
       </c>
       <c r="B79" s="1" t="n">
-        <v>43854.53472222222</v>
+        <v>43875.53472222222</v>
       </c>
       <c r="C79" t="n">
         <v>55</v>
@@ -3148,10 +3148,10 @@
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
-        <v>43854.54166666666</v>
+        <v>43875.54166666666</v>
       </c>
       <c r="B80" s="1" t="n">
-        <v>43854.54166666666</v>
+        <v>43875.54166666666</v>
       </c>
       <c r="C80" t="n">
         <v>55</v>
@@ -3183,10 +3183,10 @@
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
-        <v>43854.54861111111</v>
+        <v>43875.54861111111</v>
       </c>
       <c r="B81" s="1" t="n">
-        <v>43854.54861111111</v>
+        <v>43875.54861111111</v>
       </c>
       <c r="C81" t="n">
         <v>55</v>
@@ -3218,10 +3218,10 @@
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
-        <v>43854.55555555555</v>
+        <v>43875.55555555555</v>
       </c>
       <c r="B82" s="1" t="n">
-        <v>43854.55555555555</v>
+        <v>43875.55555555555</v>
       </c>
       <c r="C82" t="n">
         <v>55</v>
@@ -3253,10 +3253,10 @@
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
-        <v>43854.5625</v>
+        <v>43875.5625</v>
       </c>
       <c r="B83" s="1" t="n">
-        <v>43854.5625</v>
+        <v>43875.5625</v>
       </c>
       <c r="C83" t="n">
         <v>55</v>
@@ -3288,10 +3288,10 @@
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
-        <v>43854.56944444445</v>
+        <v>43875.56944444445</v>
       </c>
       <c r="B84" s="1" t="n">
-        <v>43854.56944444445</v>
+        <v>43875.56944444445</v>
       </c>
       <c r="C84" t="n">
         <v>55</v>
@@ -3323,10 +3323,10 @@
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
-        <v>43854.57638888889</v>
+        <v>43875.57638888889</v>
       </c>
       <c r="B85" s="1" t="n">
-        <v>43854.57638888889</v>
+        <v>43875.57638888889</v>
       </c>
       <c r="C85" t="n">
         <v>55</v>
@@ -3358,10 +3358,10 @@
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
-        <v>43854.58333333334</v>
+        <v>43875.58333333334</v>
       </c>
       <c r="B86" s="1" t="n">
-        <v>43854.58333333334</v>
+        <v>43875.58333333334</v>
       </c>
       <c r="C86" t="n">
         <v>55</v>
@@ -3393,10 +3393,10 @@
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
-        <v>43854.59027777778</v>
+        <v>43875.59027777778</v>
       </c>
       <c r="B87" s="1" t="n">
-        <v>43854.59027777778</v>
+        <v>43875.59027777778</v>
       </c>
       <c r="C87" t="n">
         <v>55</v>
@@ -3428,10 +3428,10 @@
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
-        <v>43854.59722222222</v>
+        <v>43875.59722222222</v>
       </c>
       <c r="B88" s="1" t="n">
-        <v>43854.59722222222</v>
+        <v>43875.59722222222</v>
       </c>
       <c r="C88" t="n">
         <v>55</v>
@@ -3463,10 +3463,10 @@
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
-        <v>43854.60416666666</v>
+        <v>43875.60416666666</v>
       </c>
       <c r="B89" s="1" t="n">
-        <v>43854.60416666666</v>
+        <v>43875.60416666666</v>
       </c>
       <c r="C89" t="n">
         <v>55</v>
@@ -3498,10 +3498,10 @@
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
-        <v>43854.61111111111</v>
+        <v>43875.61111111111</v>
       </c>
       <c r="B90" s="1" t="n">
-        <v>43854.61111111111</v>
+        <v>43875.61111111111</v>
       </c>
       <c r="C90" t="n">
         <v>55</v>
@@ -3533,10 +3533,10 @@
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
-        <v>43854.61805555555</v>
+        <v>43875.61805555555</v>
       </c>
       <c r="B91" s="1" t="n">
-        <v>43854.61805555555</v>
+        <v>43875.61805555555</v>
       </c>
       <c r="C91" t="n">
         <v>55</v>
@@ -3568,10 +3568,10 @@
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
-        <v>43854.625</v>
+        <v>43875.625</v>
       </c>
       <c r="B92" s="1" t="n">
-        <v>43854.625</v>
+        <v>43875.625</v>
       </c>
       <c r="C92" t="n">
         <v>55</v>
@@ -3603,10 +3603,10 @@
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
-        <v>43854.63194444445</v>
+        <v>43875.63194444445</v>
       </c>
       <c r="B93" s="1" t="n">
-        <v>43854.63194444445</v>
+        <v>43875.63194444445</v>
       </c>
       <c r="C93" t="n">
         <v>55</v>
@@ -3638,10 +3638,10 @@
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
-        <v>43854.63888888889</v>
+        <v>43875.63888888889</v>
       </c>
       <c r="B94" s="1" t="n">
-        <v>43854.63888888889</v>
+        <v>43875.63888888889</v>
       </c>
       <c r="C94" t="n">
         <v>55</v>
@@ -3673,10 +3673,10 @@
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
-        <v>43854.64583333334</v>
+        <v>43875.64583333334</v>
       </c>
       <c r="B95" s="1" t="n">
-        <v>43854.64583333334</v>
+        <v>43875.64583333334</v>
       </c>
       <c r="C95" t="n">
         <v>55</v>
@@ -3708,10 +3708,10 @@
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
-        <v>43854.65277777778</v>
+        <v>43875.65277777778</v>
       </c>
       <c r="B96" s="1" t="n">
-        <v>43854.65277777778</v>
+        <v>43875.65277777778</v>
       </c>
       <c r="C96" t="n">
         <v>55</v>
@@ -3743,10 +3743,10 @@
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
-        <v>43854.65972222222</v>
+        <v>43875.65972222222</v>
       </c>
       <c r="B97" s="1" t="n">
-        <v>43854.65972222222</v>
+        <v>43875.65972222222</v>
       </c>
       <c r="C97" t="n">
         <v>55</v>
@@ -3778,10 +3778,10 @@
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
-        <v>43854.66666666666</v>
+        <v>43875.66666666666</v>
       </c>
       <c r="B98" s="1" t="n">
-        <v>43854.66666666666</v>
+        <v>43875.66666666666</v>
       </c>
       <c r="C98" t="n">
         <v>55</v>
@@ -3813,10 +3813,10 @@
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
-        <v>43854.67361111111</v>
+        <v>43875.67361111111</v>
       </c>
       <c r="B99" s="1" t="n">
-        <v>43854.67361111111</v>
+        <v>43875.67361111111</v>
       </c>
       <c r="C99" t="n">
         <v>55</v>
@@ -3848,10 +3848,10 @@
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
-        <v>43854.68055555555</v>
+        <v>43875.68055555555</v>
       </c>
       <c r="B100" s="1" t="n">
-        <v>43854.68055555555</v>
+        <v>43875.68055555555</v>
       </c>
       <c r="C100" t="n">
         <v>55</v>
@@ -3883,10 +3883,10 @@
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
-        <v>43854.6875</v>
+        <v>43875.6875</v>
       </c>
       <c r="B101" s="1" t="n">
-        <v>43854.6875</v>
+        <v>43875.6875</v>
       </c>
       <c r="C101" t="n">
         <v>55</v>
@@ -3918,10 +3918,10 @@
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
-        <v>43854.69444444445</v>
+        <v>43875.69444444445</v>
       </c>
       <c r="B102" s="1" t="n">
-        <v>43854.69444444445</v>
+        <v>43875.69444444445</v>
       </c>
       <c r="C102" t="n">
         <v>55</v>
@@ -3953,10 +3953,10 @@
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
-        <v>43854.70138888889</v>
+        <v>43875.70138888889</v>
       </c>
       <c r="B103" s="1" t="n">
-        <v>43854.70138888889</v>
+        <v>43875.70138888889</v>
       </c>
       <c r="C103" t="n">
         <v>55</v>
@@ -3988,10 +3988,10 @@
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
-        <v>43854.70833333334</v>
+        <v>43875.70833333334</v>
       </c>
       <c r="B104" s="1" t="n">
-        <v>43854.70833333334</v>
+        <v>43875.70833333334</v>
       </c>
       <c r="C104" t="n">
         <v>55</v>
@@ -4023,10 +4023,10 @@
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
-        <v>43854.71527777778</v>
+        <v>43875.71527777778</v>
       </c>
       <c r="B105" s="1" t="n">
-        <v>43854.71527777778</v>
+        <v>43875.71527777778</v>
       </c>
       <c r="C105" t="n">
         <v>55</v>
@@ -4058,10 +4058,10 @@
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
-        <v>43854.72222222222</v>
+        <v>43875.72222222222</v>
       </c>
       <c r="B106" s="1" t="n">
-        <v>43854.72222222222</v>
+        <v>43875.72222222222</v>
       </c>
       <c r="C106" t="n">
         <v>55</v>
@@ -4093,10 +4093,10 @@
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
-        <v>43854.72916666666</v>
+        <v>43875.72916666666</v>
       </c>
       <c r="B107" s="1" t="n">
-        <v>43854.72916666666</v>
+        <v>43875.72916666666</v>
       </c>
       <c r="C107" t="n">
         <v>55</v>
@@ -4128,10 +4128,10 @@
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
-        <v>43854.73611111111</v>
+        <v>43875.73611111111</v>
       </c>
       <c r="B108" s="1" t="n">
-        <v>43854.73611111111</v>
+        <v>43875.73611111111</v>
       </c>
       <c r="C108" t="n">
         <v>55</v>
@@ -4163,10 +4163,10 @@
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
-        <v>43854.74305555555</v>
+        <v>43875.74305555555</v>
       </c>
       <c r="B109" s="1" t="n">
-        <v>43854.74305555555</v>
+        <v>43875.74305555555</v>
       </c>
       <c r="C109" t="n">
         <v>55</v>
@@ -4198,10 +4198,10 @@
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
-        <v>43854.75</v>
+        <v>43875.75</v>
       </c>
       <c r="B110" s="1" t="n">
-        <v>43854.75</v>
+        <v>43875.75</v>
       </c>
       <c r="C110" t="n">
         <v>55</v>
@@ -4233,10 +4233,10 @@
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
-        <v>43854.75694444445</v>
+        <v>43875.75694444445</v>
       </c>
       <c r="B111" s="1" t="n">
-        <v>43854.75694444445</v>
+        <v>43875.75694444445</v>
       </c>
       <c r="C111" t="n">
         <v>55</v>
@@ -4268,10 +4268,10 @@
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
-        <v>43854.76388888889</v>
+        <v>43875.76388888889</v>
       </c>
       <c r="B112" s="1" t="n">
-        <v>43854.76388888889</v>
+        <v>43875.76388888889</v>
       </c>
       <c r="C112" t="n">
         <v>55</v>
@@ -4303,10 +4303,10 @@
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
-        <v>43854.77083333334</v>
+        <v>43875.77083333334</v>
       </c>
       <c r="B113" s="1" t="n">
-        <v>43854.77083333334</v>
+        <v>43875.77083333334</v>
       </c>
       <c r="C113" t="n">
         <v>55</v>
@@ -4338,10 +4338,10 @@
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
-        <v>43854.77777777778</v>
+        <v>43875.77777777778</v>
       </c>
       <c r="B114" s="1" t="n">
-        <v>43854.77777777778</v>
+        <v>43875.77777777778</v>
       </c>
       <c r="C114" t="n">
         <v>55</v>
@@ -4373,10 +4373,10 @@
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
-        <v>43854.78472222222</v>
+        <v>43875.78472222222</v>
       </c>
       <c r="B115" s="1" t="n">
-        <v>43854.78472222222</v>
+        <v>43875.78472222222</v>
       </c>
       <c r="C115" t="n">
         <v>55</v>
@@ -4408,10 +4408,10 @@
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
-        <v>43854.79166666666</v>
+        <v>43875.79166666666</v>
       </c>
       <c r="B116" s="1" t="n">
-        <v>43854.79166666666</v>
+        <v>43875.79166666666</v>
       </c>
       <c r="C116" t="n">
         <v>55</v>
@@ -4443,10 +4443,10 @@
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
-        <v>43854.79861111111</v>
+        <v>43875.79861111111</v>
       </c>
       <c r="B117" s="1" t="n">
-        <v>43854.79861111111</v>
+        <v>43875.79861111111</v>
       </c>
       <c r="C117" t="n">
         <v>55</v>
@@ -4478,10 +4478,10 @@
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
-        <v>43854.80555555555</v>
+        <v>43875.80555555555</v>
       </c>
       <c r="B118" s="1" t="n">
-        <v>43854.80555555555</v>
+        <v>43875.80555555555</v>
       </c>
       <c r="C118" t="n">
         <v>55</v>
@@ -4513,10 +4513,10 @@
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
-        <v>43854.8125</v>
+        <v>43875.8125</v>
       </c>
       <c r="B119" s="1" t="n">
-        <v>43854.8125</v>
+        <v>43875.8125</v>
       </c>
       <c r="C119" t="n">
         <v>55</v>
@@ -4548,10 +4548,10 @@
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
-        <v>43854.81944444445</v>
+        <v>43875.81944444445</v>
       </c>
       <c r="B120" s="1" t="n">
-        <v>43854.81944444445</v>
+        <v>43875.81944444445</v>
       </c>
       <c r="C120" t="n">
         <v>55</v>
@@ -4583,10 +4583,10 @@
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
-        <v>43854.82638888889</v>
+        <v>43875.82638888889</v>
       </c>
       <c r="B121" s="1" t="n">
-        <v>43854.82638888889</v>
+        <v>43875.82638888889</v>
       </c>
       <c r="C121" t="n">
         <v>55</v>
@@ -4618,10 +4618,10 @@
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
-        <v>43854.83333333334</v>
+        <v>43875.83333333334</v>
       </c>
       <c r="B122" s="1" t="n">
-        <v>43854.83333333334</v>
+        <v>43875.83333333334</v>
       </c>
       <c r="C122" t="n">
         <v>55</v>
@@ -4653,10 +4653,10 @@
     </row>
     <row r="123">
       <c r="A123" s="1" t="n">
-        <v>43854.84027777778</v>
+        <v>43875.84027777778</v>
       </c>
       <c r="B123" s="1" t="n">
-        <v>43854.84027777778</v>
+        <v>43875.84027777778</v>
       </c>
       <c r="C123" t="n">
         <v>55</v>
@@ -4688,10 +4688,10 @@
     </row>
     <row r="124">
       <c r="A124" s="1" t="n">
-        <v>43854.84722222222</v>
+        <v>43875.84722222222</v>
       </c>
       <c r="B124" s="1" t="n">
-        <v>43854.84722222222</v>
+        <v>43875.84722222222</v>
       </c>
       <c r="C124" t="n">
         <v>55</v>
@@ -4723,10 +4723,10 @@
     </row>
     <row r="125">
       <c r="A125" s="1" t="n">
-        <v>43854.85416666666</v>
+        <v>43875.85416666666</v>
       </c>
       <c r="B125" s="1" t="n">
-        <v>43854.85416666666</v>
+        <v>43875.85416666666</v>
       </c>
       <c r="C125" t="n">
         <v>55</v>
@@ -4758,10 +4758,10 @@
     </row>
     <row r="126">
       <c r="A126" s="1" t="n">
-        <v>43854.86111111111</v>
+        <v>43875.86111111111</v>
       </c>
       <c r="B126" s="1" t="n">
-        <v>43854.86111111111</v>
+        <v>43875.86111111111</v>
       </c>
       <c r="C126" t="n">
         <v>55</v>
@@ -4793,10 +4793,10 @@
     </row>
     <row r="127">
       <c r="A127" s="1" t="n">
-        <v>43854.86805555555</v>
+        <v>43875.86805555555</v>
       </c>
       <c r="B127" s="1" t="n">
-        <v>43854.86805555555</v>
+        <v>43875.86805555555</v>
       </c>
       <c r="C127" t="n">
         <v>55</v>
@@ -4828,10 +4828,10 @@
     </row>
     <row r="128">
       <c r="A128" s="1" t="n">
-        <v>43854.875</v>
+        <v>43875.875</v>
       </c>
       <c r="B128" s="1" t="n">
-        <v>43854.875</v>
+        <v>43875.875</v>
       </c>
       <c r="C128" t="n">
         <v>55</v>
@@ -4863,10 +4863,10 @@
     </row>
     <row r="129">
       <c r="A129" s="1" t="n">
-        <v>43854.88194444445</v>
+        <v>43875.88194444445</v>
       </c>
       <c r="B129" s="1" t="n">
-        <v>43854.88194444445</v>
+        <v>43875.88194444445</v>
       </c>
       <c r="C129" t="n">
         <v>55</v>
@@ -4898,10 +4898,10 @@
     </row>
     <row r="130">
       <c r="A130" s="1" t="n">
-        <v>43854.88888888889</v>
+        <v>43875.88888888889</v>
       </c>
       <c r="B130" s="1" t="n">
-        <v>43854.88888888889</v>
+        <v>43875.88888888889</v>
       </c>
       <c r="C130" t="n">
         <v>55</v>
@@ -4933,10 +4933,10 @@
     </row>
     <row r="131">
       <c r="A131" s="1" t="n">
-        <v>43854.89583333334</v>
+        <v>43875.89583333334</v>
       </c>
       <c r="B131" s="1" t="n">
-        <v>43854.89583333334</v>
+        <v>43875.89583333334</v>
       </c>
       <c r="C131" t="n">
         <v>55</v>
@@ -4968,10 +4968,10 @@
     </row>
     <row r="132">
       <c r="A132" s="1" t="n">
-        <v>43854.90277777778</v>
+        <v>43875.90277777778</v>
       </c>
       <c r="B132" s="1" t="n">
-        <v>43854.90277777778</v>
+        <v>43875.90277777778</v>
       </c>
       <c r="C132" t="n">
         <v>55</v>
@@ -5003,10 +5003,10 @@
     </row>
     <row r="133">
       <c r="A133" s="1" t="n">
-        <v>43854.90972222222</v>
+        <v>43875.90972222222</v>
       </c>
       <c r="B133" s="1" t="n">
-        <v>43854.90972222222</v>
+        <v>43875.90972222222</v>
       </c>
       <c r="C133" t="n">
         <v>55</v>
@@ -5038,10 +5038,10 @@
     </row>
     <row r="134">
       <c r="A134" s="1" t="n">
-        <v>43854.91666666666</v>
+        <v>43875.91666666666</v>
       </c>
       <c r="B134" s="1" t="n">
-        <v>43854.91666666666</v>
+        <v>43875.91666666666</v>
       </c>
       <c r="C134" t="n">
         <v>55</v>
@@ -5073,10 +5073,10 @@
     </row>
     <row r="135">
       <c r="A135" s="1" t="n">
-        <v>43854.92361111111</v>
+        <v>43875.92361111111</v>
       </c>
       <c r="B135" s="1" t="n">
-        <v>43854.92361111111</v>
+        <v>43875.92361111111</v>
       </c>
       <c r="C135" t="n">
         <v>55</v>
@@ -5108,10 +5108,10 @@
     </row>
     <row r="136">
       <c r="A136" s="1" t="n">
-        <v>43854.93055555555</v>
+        <v>43875.93055555555</v>
       </c>
       <c r="B136" s="1" t="n">
-        <v>43854.93055555555</v>
+        <v>43875.93055555555</v>
       </c>
       <c r="C136" t="n">
         <v>55</v>
@@ -5143,10 +5143,10 @@
     </row>
     <row r="137">
       <c r="A137" s="1" t="n">
-        <v>43854.9375</v>
+        <v>43875.9375</v>
       </c>
       <c r="B137" s="1" t="n">
-        <v>43854.9375</v>
+        <v>43875.9375</v>
       </c>
       <c r="C137" t="n">
         <v>55</v>
@@ -5178,10 +5178,10 @@
     </row>
     <row r="138">
       <c r="A138" s="1" t="n">
-        <v>43854.94444444445</v>
+        <v>43875.94444444445</v>
       </c>
       <c r="B138" s="1" t="n">
-        <v>43854.94444444445</v>
+        <v>43875.94444444445</v>
       </c>
       <c r="C138" t="n">
         <v>55</v>
@@ -5213,10 +5213,10 @@
     </row>
     <row r="139">
       <c r="A139" s="1" t="n">
-        <v>43854.95138888889</v>
+        <v>43875.95138888889</v>
       </c>
       <c r="B139" s="1" t="n">
-        <v>43854.95138888889</v>
+        <v>43875.95138888889</v>
       </c>
       <c r="C139" t="n">
         <v>55</v>
@@ -5248,10 +5248,10 @@
     </row>
     <row r="140">
       <c r="A140" s="1" t="n">
-        <v>43854.95833333334</v>
+        <v>43875.95833333334</v>
       </c>
       <c r="B140" s="1" t="n">
-        <v>43854.95833333334</v>
+        <v>43875.95833333334</v>
       </c>
       <c r="C140" t="n">
         <v>55</v>
@@ -5283,10 +5283,10 @@
     </row>
     <row r="141">
       <c r="A141" s="1" t="n">
-        <v>43854.96527777778</v>
+        <v>43875.96527777778</v>
       </c>
       <c r="B141" s="1" t="n">
-        <v>43854.96527777778</v>
+        <v>43875.96527777778</v>
       </c>
       <c r="C141" t="n">
         <v>55</v>
@@ -5318,10 +5318,10 @@
     </row>
     <row r="142">
       <c r="A142" s="1" t="n">
-        <v>43854.97222222222</v>
+        <v>43875.97222222222</v>
       </c>
       <c r="B142" s="1" t="n">
-        <v>43854.97222222222</v>
+        <v>43875.97222222222</v>
       </c>
       <c r="C142" t="n">
         <v>55</v>
@@ -5353,10 +5353,10 @@
     </row>
     <row r="143">
       <c r="A143" s="1" t="n">
-        <v>43854.97916666666</v>
+        <v>43875.97916666666</v>
       </c>
       <c r="B143" s="1" t="n">
-        <v>43854.97916666666</v>
+        <v>43875.97916666666</v>
       </c>
       <c r="C143" t="n">
         <v>55</v>
@@ -5388,10 +5388,10 @@
     </row>
     <row r="144">
       <c r="A144" s="1" t="n">
-        <v>43854.98611111111</v>
+        <v>43875.98611111111</v>
       </c>
       <c r="B144" s="1" t="n">
-        <v>43854.98611111111</v>
+        <v>43875.98611111111</v>
       </c>
       <c r="C144" t="n">
         <v>55</v>
@@ -5423,10 +5423,10 @@
     </row>
     <row r="145">
       <c r="A145" s="1" t="n">
-        <v>43854.99305555555</v>
+        <v>43875.99305555555</v>
       </c>
       <c r="B145" s="1" t="n">
-        <v>43854.99305555555</v>
+        <v>43875.99305555555</v>
       </c>
       <c r="C145" t="n">
         <v>55</v>
@@ -5458,10 +5458,10 @@
     </row>
     <row r="146">
       <c r="A146" s="1" t="n">
-        <v>43855</v>
+        <v>43876</v>
       </c>
       <c r="B146" s="1" t="n">
-        <v>43855</v>
+        <v>43876</v>
       </c>
       <c r="C146" t="n">
         <v>55</v>
@@ -5493,10 +5493,10 @@
     </row>
     <row r="147">
       <c r="A147" s="1" t="n">
-        <v>43855.00694444445</v>
+        <v>43876.00694444445</v>
       </c>
       <c r="B147" s="1" t="n">
-        <v>43855.00694444445</v>
+        <v>43876.00694444445</v>
       </c>
       <c r="C147" t="n">
         <v>55</v>
@@ -5528,10 +5528,10 @@
     </row>
     <row r="148">
       <c r="A148" s="1" t="n">
-        <v>43855.01388888889</v>
+        <v>43876.01388888889</v>
       </c>
       <c r="B148" s="1" t="n">
-        <v>43855.01388888889</v>
+        <v>43876.01388888889</v>
       </c>
       <c r="C148" t="n">
         <v>55</v>
@@ -5563,10 +5563,10 @@
     </row>
     <row r="149">
       <c r="A149" s="1" t="n">
-        <v>43855.02083333334</v>
+        <v>43876.02083333334</v>
       </c>
       <c r="B149" s="1" t="n">
-        <v>43855.02083333334</v>
+        <v>43876.02083333334</v>
       </c>
       <c r="C149" t="n">
         <v>55</v>
@@ -5598,10 +5598,10 @@
     </row>
     <row r="150">
       <c r="A150" s="1" t="n">
-        <v>43855.02777777778</v>
+        <v>43876.02777777778</v>
       </c>
       <c r="B150" s="1" t="n">
-        <v>43855.02777777778</v>
+        <v>43876.02777777778</v>
       </c>
       <c r="C150" t="n">
         <v>55</v>
@@ -5633,10 +5633,10 @@
     </row>
     <row r="151">
       <c r="A151" s="1" t="n">
-        <v>43855.03472222222</v>
+        <v>43876.03472222222</v>
       </c>
       <c r="B151" s="1" t="n">
-        <v>43855.03472222222</v>
+        <v>43876.03472222222</v>
       </c>
       <c r="C151" t="n">
         <v>55</v>
@@ -5668,10 +5668,10 @@
     </row>
     <row r="152">
       <c r="A152" s="1" t="n">
-        <v>43855.04166666666</v>
+        <v>43876.04166666666</v>
       </c>
       <c r="B152" s="1" t="n">
-        <v>43855.04166666666</v>
+        <v>43876.04166666666</v>
       </c>
       <c r="C152" t="n">
         <v>55</v>
@@ -5703,10 +5703,10 @@
     </row>
     <row r="153">
       <c r="A153" s="1" t="n">
-        <v>43855.04861111111</v>
+        <v>43876.04861111111</v>
       </c>
       <c r="B153" s="1" t="n">
-        <v>43855.04861111111</v>
+        <v>43876.04861111111</v>
       </c>
       <c r="C153" t="n">
         <v>55</v>
@@ -5738,10 +5738,10 @@
     </row>
     <row r="154">
       <c r="A154" s="1" t="n">
-        <v>43855.05555555555</v>
+        <v>43876.05555555555</v>
       </c>
       <c r="B154" s="1" t="n">
-        <v>43855.05555555555</v>
+        <v>43876.05555555555</v>
       </c>
       <c r="C154" t="n">
         <v>55</v>
@@ -5773,10 +5773,10 @@
     </row>
     <row r="155">
       <c r="A155" s="1" t="n">
-        <v>43855.0625</v>
+        <v>43876.0625</v>
       </c>
       <c r="B155" s="1" t="n">
-        <v>43855.0625</v>
+        <v>43876.0625</v>
       </c>
       <c r="C155" t="n">
         <v>55</v>
@@ -5808,10 +5808,10 @@
     </row>
     <row r="156">
       <c r="A156" s="1" t="n">
-        <v>43855.06944444445</v>
+        <v>43876.06944444445</v>
       </c>
       <c r="B156" s="1" t="n">
-        <v>43855.06944444445</v>
+        <v>43876.06944444445</v>
       </c>
       <c r="C156" t="n">
         <v>55</v>
@@ -5843,10 +5843,10 @@
     </row>
     <row r="157">
       <c r="A157" s="1" t="n">
-        <v>43855.07638888889</v>
+        <v>43876.07638888889</v>
       </c>
       <c r="B157" s="1" t="n">
-        <v>43855.07638888889</v>
+        <v>43876.07638888889</v>
       </c>
       <c r="C157" t="n">
         <v>55</v>
@@ -5878,10 +5878,10 @@
     </row>
     <row r="158">
       <c r="A158" s="1" t="n">
-        <v>43855.08333333334</v>
+        <v>43876.08333333334</v>
       </c>
       <c r="B158" s="1" t="n">
-        <v>43855.08333333334</v>
+        <v>43876.08333333334</v>
       </c>
       <c r="C158" t="n">
         <v>55</v>
@@ -5913,10 +5913,10 @@
     </row>
     <row r="159">
       <c r="A159" s="1" t="n">
-        <v>43855.09027777778</v>
+        <v>43876.09027777778</v>
       </c>
       <c r="B159" s="1" t="n">
-        <v>43855.09027777778</v>
+        <v>43876.09027777778</v>
       </c>
       <c r="C159" t="n">
         <v>55</v>
@@ -5948,10 +5948,10 @@
     </row>
     <row r="160">
       <c r="A160" s="1" t="n">
-        <v>43855.09722222222</v>
+        <v>43876.09722222222</v>
       </c>
       <c r="B160" s="1" t="n">
-        <v>43855.09722222222</v>
+        <v>43876.09722222222</v>
       </c>
       <c r="C160" t="n">
         <v>55</v>
@@ -5983,10 +5983,10 @@
     </row>
     <row r="161">
       <c r="A161" s="1" t="n">
-        <v>43855.10416666666</v>
+        <v>43876.10416666666</v>
       </c>
       <c r="B161" s="1" t="n">
-        <v>43855.10416666666</v>
+        <v>43876.10416666666</v>
       </c>
       <c r="C161" t="n">
         <v>55</v>
@@ -6018,10 +6018,10 @@
     </row>
     <row r="162">
       <c r="A162" s="1" t="n">
-        <v>43855.11111111111</v>
+        <v>43876.11111111111</v>
       </c>
       <c r="B162" s="1" t="n">
-        <v>43855.11111111111</v>
+        <v>43876.11111111111</v>
       </c>
       <c r="C162" t="n">
         <v>55</v>
@@ -6053,10 +6053,10 @@
     </row>
     <row r="163">
       <c r="A163" s="1" t="n">
-        <v>43855.11805555555</v>
+        <v>43876.11805555555</v>
       </c>
       <c r="B163" s="1" t="n">
-        <v>43855.11805555555</v>
+        <v>43876.11805555555</v>
       </c>
       <c r="C163" t="n">
         <v>55</v>
@@ -6088,10 +6088,10 @@
     </row>
     <row r="164">
       <c r="A164" s="1" t="n">
-        <v>43855.125</v>
+        <v>43876.125</v>
       </c>
       <c r="B164" s="1" t="n">
-        <v>43855.125</v>
+        <v>43876.125</v>
       </c>
       <c r="C164" t="n">
         <v>55</v>
@@ -6123,10 +6123,10 @@
     </row>
     <row r="165">
       <c r="A165" s="1" t="n">
-        <v>43855.13194444445</v>
+        <v>43876.13194444445</v>
       </c>
       <c r="B165" s="1" t="n">
-        <v>43855.13194444445</v>
+        <v>43876.13194444445</v>
       </c>
       <c r="C165" t="n">
         <v>55</v>
@@ -6158,10 +6158,10 @@
     </row>
     <row r="166">
       <c r="A166" s="1" t="n">
-        <v>43855.13888888889</v>
+        <v>43876.13888888889</v>
       </c>
       <c r="B166" s="1" t="n">
-        <v>43855.13888888889</v>
+        <v>43876.13888888889</v>
       </c>
       <c r="C166" t="n">
         <v>55</v>
@@ -6193,10 +6193,10 @@
     </row>
     <row r="167">
       <c r="A167" s="1" t="n">
-        <v>43855.14583333334</v>
+        <v>43876.14583333334</v>
       </c>
       <c r="B167" s="1" t="n">
-        <v>43855.14583333334</v>
+        <v>43876.14583333334</v>
       </c>
       <c r="C167" t="n">
         <v>55</v>
@@ -6228,10 +6228,10 @@
     </row>
     <row r="168">
       <c r="A168" s="1" t="n">
-        <v>43855.15277777778</v>
+        <v>43876.15277777778</v>
       </c>
       <c r="B168" s="1" t="n">
-        <v>43855.15277777778</v>
+        <v>43876.15277777778</v>
       </c>
       <c r="C168" t="n">
         <v>55</v>
@@ -6263,10 +6263,10 @@
     </row>
     <row r="169">
       <c r="A169" s="1" t="n">
-        <v>43855.15972222222</v>
+        <v>43876.15972222222</v>
       </c>
       <c r="B169" s="1" t="n">
-        <v>43855.15972222222</v>
+        <v>43876.15972222222</v>
       </c>
       <c r="C169" t="n">
         <v>55</v>
@@ -6298,10 +6298,10 @@
     </row>
     <row r="170">
       <c r="A170" s="1" t="n">
-        <v>43855.16666666666</v>
+        <v>43876.16666666666</v>
       </c>
       <c r="B170" s="1" t="n">
-        <v>43855.16666666666</v>
+        <v>43876.16666666666</v>
       </c>
       <c r="C170" t="n">
         <v>55</v>
@@ -6333,10 +6333,10 @@
     </row>
     <row r="171">
       <c r="A171" s="1" t="n">
-        <v>43855.17361111111</v>
+        <v>43876.17361111111</v>
       </c>
       <c r="B171" s="1" t="n">
-        <v>43855.17361111111</v>
+        <v>43876.17361111111</v>
       </c>
       <c r="C171" t="n">
         <v>55</v>
@@ -6368,10 +6368,10 @@
     </row>
     <row r="172">
       <c r="A172" s="1" t="n">
-        <v>43855.18055555555</v>
+        <v>43876.18055555555</v>
       </c>
       <c r="B172" s="1" t="n">
-        <v>43855.18055555555</v>
+        <v>43876.18055555555</v>
       </c>
       <c r="C172" t="n">
         <v>55</v>
@@ -6403,10 +6403,10 @@
     </row>
     <row r="173">
       <c r="A173" s="1" t="n">
-        <v>43855.1875</v>
+        <v>43876.1875</v>
       </c>
       <c r="B173" s="1" t="n">
-        <v>43855.1875</v>
+        <v>43876.1875</v>
       </c>
       <c r="C173" t="n">
         <v>55</v>
@@ -6438,10 +6438,10 @@
     </row>
     <row r="174">
       <c r="A174" s="1" t="n">
-        <v>43855.19444444445</v>
+        <v>43876.19444444445</v>
       </c>
       <c r="B174" s="1" t="n">
-        <v>43855.19444444445</v>
+        <v>43876.19444444445</v>
       </c>
       <c r="C174" t="n">
         <v>55</v>
@@ -6473,10 +6473,10 @@
     </row>
     <row r="175">
       <c r="A175" s="1" t="n">
-        <v>43855.20138888889</v>
+        <v>43876.20138888889</v>
       </c>
       <c r="B175" s="1" t="n">
-        <v>43855.20138888889</v>
+        <v>43876.20138888889</v>
       </c>
       <c r="C175" t="n">
         <v>55</v>
@@ -6508,10 +6508,10 @@
     </row>
     <row r="176">
       <c r="A176" s="1" t="n">
-        <v>43855.20833333334</v>
+        <v>43876.20833333334</v>
       </c>
       <c r="B176" s="1" t="n">
-        <v>43855.20833333334</v>
+        <v>43876.20833333334</v>
       </c>
       <c r="C176" t="n">
         <v>55</v>
@@ -6543,10 +6543,10 @@
     </row>
     <row r="177">
       <c r="A177" s="1" t="n">
-        <v>43855.21527777778</v>
+        <v>43876.21527777778</v>
       </c>
       <c r="B177" s="1" t="n">
-        <v>43855.21527777778</v>
+        <v>43876.21527777778</v>
       </c>
       <c r="C177" t="n">
         <v>55</v>
@@ -6578,10 +6578,10 @@
     </row>
     <row r="178">
       <c r="A178" s="1" t="n">
-        <v>43855.22222222222</v>
+        <v>43876.22222222222</v>
       </c>
       <c r="B178" s="1" t="n">
-        <v>43855.22222222222</v>
+        <v>43876.22222222222</v>
       </c>
       <c r="C178" t="n">
         <v>55</v>
@@ -6613,10 +6613,10 @@
     </row>
     <row r="179">
       <c r="A179" s="1" t="n">
-        <v>43855.22916666666</v>
+        <v>43876.22916666666</v>
       </c>
       <c r="B179" s="1" t="n">
-        <v>43855.22916666666</v>
+        <v>43876.22916666666</v>
       </c>
       <c r="C179" t="n">
         <v>55</v>
@@ -6648,10 +6648,10 @@
     </row>
     <row r="180">
       <c r="A180" s="1" t="n">
-        <v>43855.23611111111</v>
+        <v>43876.23611111111</v>
       </c>
       <c r="B180" s="1" t="n">
-        <v>43855.23611111111</v>
+        <v>43876.23611111111</v>
       </c>
       <c r="C180" t="n">
         <v>55</v>
@@ -6683,10 +6683,10 @@
     </row>
     <row r="181">
       <c r="A181" s="1" t="n">
-        <v>43855.24305555555</v>
+        <v>43876.24305555555</v>
       </c>
       <c r="B181" s="1" t="n">
-        <v>43855.24305555555</v>
+        <v>43876.24305555555</v>
       </c>
       <c r="C181" t="n">
         <v>55</v>
@@ -6718,10 +6718,10 @@
     </row>
     <row r="182">
       <c r="A182" s="1" t="n">
-        <v>43855.25</v>
+        <v>43876.25</v>
       </c>
       <c r="B182" s="1" t="n">
-        <v>43855.25</v>
+        <v>43876.25</v>
       </c>
       <c r="C182" t="n">
         <v>55</v>
@@ -6753,10 +6753,10 @@
     </row>
     <row r="183">
       <c r="A183" s="1" t="n">
-        <v>43855.25694444445</v>
+        <v>43876.25694444445</v>
       </c>
       <c r="B183" s="1" t="n">
-        <v>43855.25694444445</v>
+        <v>43876.25694444445</v>
       </c>
       <c r="C183" t="n">
         <v>55</v>
@@ -6788,10 +6788,10 @@
     </row>
     <row r="184">
       <c r="A184" s="1" t="n">
-        <v>43855.26388888889</v>
+        <v>43876.26388888889</v>
       </c>
       <c r="B184" s="1" t="n">
-        <v>43855.26388888889</v>
+        <v>43876.26388888889</v>
       </c>
       <c r="C184" t="n">
         <v>55</v>
@@ -6823,10 +6823,10 @@
     </row>
     <row r="185">
       <c r="A185" s="1" t="n">
-        <v>43855.27083333334</v>
+        <v>43876.27083333334</v>
       </c>
       <c r="B185" s="1" t="n">
-        <v>43855.27083333334</v>
+        <v>43876.27083333334</v>
       </c>
       <c r="C185" t="n">
         <v>55</v>
@@ -6858,10 +6858,10 @@
     </row>
     <row r="186">
       <c r="A186" s="1" t="n">
-        <v>43855.27777777778</v>
+        <v>43876.27777777778</v>
       </c>
       <c r="B186" s="1" t="n">
-        <v>43855.27777777778</v>
+        <v>43876.27777777778</v>
       </c>
       <c r="C186" t="n">
         <v>55</v>
@@ -6893,10 +6893,10 @@
     </row>
     <row r="187">
       <c r="A187" s="1" t="n">
-        <v>43855.28472222222</v>
+        <v>43876.28472222222</v>
       </c>
       <c r="B187" s="1" t="n">
-        <v>43855.28472222222</v>
+        <v>43876.28472222222</v>
       </c>
       <c r="C187" t="n">
         <v>55</v>
@@ -6928,10 +6928,10 @@
     </row>
     <row r="188">
       <c r="A188" s="1" t="n">
-        <v>43855.29166666666</v>
+        <v>43876.29166666666</v>
       </c>
       <c r="B188" s="1" t="n">
-        <v>43855.29166666666</v>
+        <v>43876.29166666666</v>
       </c>
       <c r="C188" t="n">
         <v>55</v>
@@ -6963,10 +6963,10 @@
     </row>
     <row r="189">
       <c r="A189" s="1" t="n">
-        <v>43855.29861111111</v>
+        <v>43876.29861111111</v>
       </c>
       <c r="B189" s="1" t="n">
-        <v>43855.29861111111</v>
+        <v>43876.29861111111</v>
       </c>
       <c r="C189" t="n">
         <v>55</v>
@@ -6998,10 +6998,10 @@
     </row>
     <row r="190">
       <c r="A190" s="1" t="n">
-        <v>43855.30555555555</v>
+        <v>43876.30555555555</v>
       </c>
       <c r="B190" s="1" t="n">
-        <v>43855.30555555555</v>
+        <v>43876.30555555555</v>
       </c>
       <c r="C190" t="n">
         <v>55</v>
@@ -7033,10 +7033,10 @@
     </row>
     <row r="191">
       <c r="A191" s="1" t="n">
-        <v>43855.3125</v>
+        <v>43876.3125</v>
       </c>
       <c r="B191" s="1" t="n">
-        <v>43855.3125</v>
+        <v>43876.3125</v>
       </c>
       <c r="C191" t="n">
         <v>55</v>
@@ -7068,10 +7068,10 @@
     </row>
     <row r="192">
       <c r="A192" s="1" t="n">
-        <v>43855.31944444445</v>
+        <v>43876.31944444445</v>
       </c>
       <c r="B192" s="1" t="n">
-        <v>43855.31944444445</v>
+        <v>43876.31944444445</v>
       </c>
       <c r="C192" t="n">
         <v>55</v>
@@ -7103,10 +7103,10 @@
     </row>
     <row r="193">
       <c r="A193" s="1" t="n">
-        <v>43855.32638888889</v>
+        <v>43876.32638888889</v>
       </c>
       <c r="B193" s="1" t="n">
-        <v>43855.32638888889</v>
+        <v>43876.32638888889</v>
       </c>
       <c r="C193" t="n">
         <v>55</v>
@@ -7138,10 +7138,10 @@
     </row>
     <row r="194">
       <c r="A194" s="1" t="n">
-        <v>43855.33333333334</v>
+        <v>43876.33333333334</v>
       </c>
       <c r="B194" s="1" t="n">
-        <v>43855.33333333334</v>
+        <v>43876.33333333334</v>
       </c>
       <c r="C194" t="n">
         <v>55</v>
@@ -7173,10 +7173,10 @@
     </row>
     <row r="195">
       <c r="A195" s="1" t="n">
-        <v>43855.34027777778</v>
+        <v>43876.34027777778</v>
       </c>
       <c r="B195" s="1" t="n">
-        <v>43855.34027777778</v>
+        <v>43876.34027777778</v>
       </c>
       <c r="C195" t="n">
         <v>55</v>
@@ -7208,10 +7208,10 @@
     </row>
     <row r="196">
       <c r="A196" s="1" t="n">
-        <v>43855.34722222222</v>
+        <v>43876.34722222222</v>
       </c>
       <c r="B196" s="1" t="n">
-        <v>43855.34722222222</v>
+        <v>43876.34722222222</v>
       </c>
       <c r="C196" t="n">
         <v>55</v>
@@ -7243,10 +7243,10 @@
     </row>
     <row r="197">
       <c r="A197" s="1" t="n">
-        <v>43855.35416666666</v>
+        <v>43876.35416666666</v>
       </c>
       <c r="B197" s="1" t="n">
-        <v>43855.35416666666</v>
+        <v>43876.35416666666</v>
       </c>
       <c r="C197" t="n">
         <v>55</v>
@@ -7278,10 +7278,10 @@
     </row>
     <row r="198">
       <c r="A198" s="1" t="n">
-        <v>43855.36111111111</v>
+        <v>43876.36111111111</v>
       </c>
       <c r="B198" s="1" t="n">
-        <v>43855.36111111111</v>
+        <v>43876.36111111111</v>
       </c>
       <c r="C198" t="n">
         <v>55</v>
@@ -7313,10 +7313,10 @@
     </row>
     <row r="199">
       <c r="A199" s="1" t="n">
-        <v>43855.36805555555</v>
+        <v>43876.36805555555</v>
       </c>
       <c r="B199" s="1" t="n">
-        <v>43855.36805555555</v>
+        <v>43876.36805555555</v>
       </c>
       <c r="C199" t="n">
         <v>55</v>
@@ -7348,10 +7348,10 @@
     </row>
     <row r="200">
       <c r="A200" s="1" t="n">
-        <v>43855.375</v>
+        <v>43876.375</v>
       </c>
       <c r="B200" s="1" t="n">
-        <v>43855.375</v>
+        <v>43876.375</v>
       </c>
       <c r="C200" t="n">
         <v>55</v>
@@ -7383,10 +7383,10 @@
     </row>
     <row r="201">
       <c r="A201" s="1" t="n">
-        <v>43855.38194444445</v>
+        <v>43876.38194444445</v>
       </c>
       <c r="B201" s="1" t="n">
-        <v>43855.38194444445</v>
+        <v>43876.38194444445</v>
       </c>
       <c r="C201" t="n">
         <v>55</v>
@@ -7418,10 +7418,10 @@
     </row>
     <row r="202">
       <c r="A202" s="1" t="n">
-        <v>43855.38888888889</v>
+        <v>43876.38888888889</v>
       </c>
       <c r="B202" s="1" t="n">
-        <v>43855.38888888889</v>
+        <v>43876.38888888889</v>
       </c>
       <c r="C202" t="n">
         <v>55</v>
@@ -7453,10 +7453,10 @@
     </row>
     <row r="203">
       <c r="A203" s="1" t="n">
-        <v>43855.39583333334</v>
+        <v>43876.39583333334</v>
       </c>
       <c r="B203" s="1" t="n">
-        <v>43855.39583333334</v>
+        <v>43876.39583333334</v>
       </c>
       <c r="C203" t="n">
         <v>55</v>
@@ -7488,10 +7488,10 @@
     </row>
     <row r="204">
       <c r="A204" s="1" t="n">
-        <v>43855.40277777778</v>
+        <v>43876.40277777778</v>
       </c>
       <c r="B204" s="1" t="n">
-        <v>43855.40277777778</v>
+        <v>43876.40277777778</v>
       </c>
       <c r="C204" t="n">
         <v>55</v>
@@ -7523,10 +7523,10 @@
     </row>
     <row r="205">
       <c r="A205" s="1" t="n">
-        <v>43855.40972222222</v>
+        <v>43876.40972222222</v>
       </c>
       <c r="B205" s="1" t="n">
-        <v>43855.40972222222</v>
+        <v>43876.40972222222</v>
       </c>
       <c r="C205" t="n">
         <v>55</v>
@@ -7558,10 +7558,10 @@
     </row>
     <row r="206">
       <c r="A206" s="1" t="n">
-        <v>43855.41666666666</v>
+        <v>43876.41666666666</v>
       </c>
       <c r="B206" s="1" t="n">
-        <v>43855.41666666666</v>
+        <v>43876.41666666666</v>
       </c>
       <c r="C206" t="n">
         <v>55</v>
@@ -7593,10 +7593,10 @@
     </row>
     <row r="207">
       <c r="A207" s="1" t="n">
-        <v>43855.42361111111</v>
+        <v>43876.42361111111</v>
       </c>
       <c r="B207" s="1" t="n">
-        <v>43855.42361111111</v>
+        <v>43876.42361111111</v>
       </c>
       <c r="C207" t="n">
         <v>55</v>
@@ -7628,10 +7628,10 @@
     </row>
     <row r="208">
       <c r="A208" s="1" t="n">
-        <v>43855.43055555555</v>
+        <v>43876.43055555555</v>
       </c>
       <c r="B208" s="1" t="n">
-        <v>43855.43055555555</v>
+        <v>43876.43055555555</v>
       </c>
       <c r="C208" t="n">
         <v>55</v>
@@ -7663,10 +7663,10 @@
     </row>
     <row r="209">
       <c r="A209" s="1" t="n">
-        <v>43855.4375</v>
+        <v>43876.4375</v>
       </c>
       <c r="B209" s="1" t="n">
-        <v>43855.4375</v>
+        <v>43876.4375</v>
       </c>
       <c r="C209" t="n">
         <v>55</v>
@@ -7698,10 +7698,10 @@
     </row>
     <row r="210">
       <c r="A210" s="1" t="n">
-        <v>43855.44444444445</v>
+        <v>43876.44444444445</v>
       </c>
       <c r="B210" s="1" t="n">
-        <v>43855.44444444445</v>
+        <v>43876.44444444445</v>
       </c>
       <c r="C210" t="n">
         <v>55</v>
@@ -7733,10 +7733,10 @@
     </row>
     <row r="211">
       <c r="A211" s="1" t="n">
-        <v>43855.45138888889</v>
+        <v>43876.45138888889</v>
       </c>
       <c r="B211" s="1" t="n">
-        <v>43855.45138888889</v>
+        <v>43876.45138888889</v>
       </c>
       <c r="C211" t="n">
         <v>55</v>
@@ -7768,10 +7768,10 @@
     </row>
     <row r="212">
       <c r="A212" s="1" t="n">
-        <v>43855.45833333334</v>
+        <v>43876.45833333334</v>
       </c>
       <c r="B212" s="1" t="n">
-        <v>43855.45833333334</v>
+        <v>43876.45833333334</v>
       </c>
       <c r="C212" t="n">
         <v>55</v>
@@ -7803,10 +7803,10 @@
     </row>
     <row r="213">
       <c r="A213" s="1" t="n">
-        <v>43855.46527777778</v>
+        <v>43876.46527777778</v>
       </c>
       <c r="B213" s="1" t="n">
-        <v>43855.46527777778</v>
+        <v>43876.46527777778</v>
       </c>
       <c r="C213" t="n">
         <v>55</v>
@@ -7838,10 +7838,10 @@
     </row>
     <row r="214">
       <c r="A214" s="1" t="n">
-        <v>43855.47222222222</v>
+        <v>43876.47222222222</v>
       </c>
       <c r="B214" s="1" t="n">
-        <v>43855.47222222222</v>
+        <v>43876.47222222222</v>
       </c>
       <c r="C214" t="n">
         <v>55</v>
@@ -7873,10 +7873,10 @@
     </row>
     <row r="215">
       <c r="A215" s="1" t="n">
-        <v>43855.47916666666</v>
+        <v>43876.47916666666</v>
       </c>
       <c r="B215" s="1" t="n">
-        <v>43855.47916666666</v>
+        <v>43876.47916666666</v>
       </c>
       <c r="C215" t="n">
         <v>55</v>
@@ -7908,10 +7908,10 @@
     </row>
     <row r="216">
       <c r="A216" s="1" t="n">
-        <v>43855.48611111111</v>
+        <v>43876.48611111111</v>
       </c>
       <c r="B216" s="1" t="n">
-        <v>43855.48611111111</v>
+        <v>43876.48611111111</v>
       </c>
       <c r="C216" t="n">
         <v>55</v>
@@ -7943,10 +7943,10 @@
     </row>
     <row r="217">
       <c r="A217" s="1" t="n">
-        <v>43855.49305555555</v>
+        <v>43876.49305555555</v>
       </c>
       <c r="B217" s="1" t="n">
-        <v>43855.49305555555</v>
+        <v>43876.49305555555</v>
       </c>
       <c r="C217" t="n">
         <v>55</v>
@@ -7978,10 +7978,10 @@
     </row>
     <row r="218">
       <c r="A218" s="1" t="n">
-        <v>43855.5</v>
+        <v>43876.5</v>
       </c>
       <c r="B218" s="1" t="n">
-        <v>43855.5</v>
+        <v>43876.5</v>
       </c>
       <c r="C218" t="n">
         <v>55</v>
@@ -8013,10 +8013,10 @@
     </row>
     <row r="219">
       <c r="A219" s="1" t="n">
-        <v>43855.50694444445</v>
+        <v>43876.50694444445</v>
       </c>
       <c r="B219" s="1" t="n">
-        <v>43855.50694444445</v>
+        <v>43876.50694444445</v>
       </c>
       <c r="C219" t="n">
         <v>55</v>
@@ -8048,10 +8048,10 @@
     </row>
     <row r="220">
       <c r="A220" s="1" t="n">
-        <v>43855.51388888889</v>
+        <v>43876.51388888889</v>
       </c>
       <c r="B220" s="1" t="n">
-        <v>43855.51388888889</v>
+        <v>43876.51388888889</v>
       </c>
       <c r="C220" t="n">
         <v>55</v>
@@ -8083,10 +8083,10 @@
     </row>
     <row r="221">
       <c r="A221" s="1" t="n">
-        <v>43855.52083333334</v>
+        <v>43876.52083333334</v>
       </c>
       <c r="B221" s="1" t="n">
-        <v>43855.52083333334</v>
+        <v>43876.52083333334</v>
       </c>
       <c r="C221" t="n">
         <v>55</v>
@@ -8118,10 +8118,10 @@
     </row>
     <row r="222">
       <c r="A222" s="1" t="n">
-        <v>43855.52777777778</v>
+        <v>43876.52777777778</v>
       </c>
       <c r="B222" s="1" t="n">
-        <v>43855.52777777778</v>
+        <v>43876.52777777778</v>
       </c>
       <c r="C222" t="n">
         <v>55</v>
@@ -8153,10 +8153,10 @@
     </row>
     <row r="223">
       <c r="A223" s="1" t="n">
-        <v>43855.53472222222</v>
+        <v>43876.53472222222</v>
       </c>
       <c r="B223" s="1" t="n">
-        <v>43855.53472222222</v>
+        <v>43876.53472222222</v>
       </c>
       <c r="C223" t="n">
         <v>55</v>
@@ -8188,10 +8188,10 @@
     </row>
     <row r="224">
       <c r="A224" s="1" t="n">
-        <v>43855.54166666666</v>
+        <v>43876.54166666666</v>
       </c>
       <c r="B224" s="1" t="n">
-        <v>43855.54166666666</v>
+        <v>43876.54166666666</v>
       </c>
       <c r="C224" t="n">
         <v>55</v>
@@ -8223,10 +8223,10 @@
     </row>
     <row r="225">
       <c r="A225" s="1" t="n">
-        <v>43855.54861111111</v>
+        <v>43876.54861111111</v>
       </c>
       <c r="B225" s="1" t="n">
-        <v>43855.54861111111</v>
+        <v>43876.54861111111</v>
       </c>
       <c r="C225" t="n">
         <v>55</v>
@@ -8258,10 +8258,10 @@
     </row>
     <row r="226">
       <c r="A226" s="1" t="n">
-        <v>43855.55555555555</v>
+        <v>43876.55555555555</v>
       </c>
       <c r="B226" s="1" t="n">
-        <v>43855.55555555555</v>
+        <v>43876.55555555555</v>
       </c>
       <c r="C226" t="n">
         <v>55</v>
@@ -8293,10 +8293,10 @@
     </row>
     <row r="227">
       <c r="A227" s="1" t="n">
-        <v>43855.5625</v>
+        <v>43876.5625</v>
       </c>
       <c r="B227" s="1" t="n">
-        <v>43855.5625</v>
+        <v>43876.5625</v>
       </c>
       <c r="C227" t="n">
         <v>55</v>
@@ -8328,10 +8328,10 @@
     </row>
     <row r="228">
       <c r="A228" s="1" t="n">
-        <v>43855.56944444445</v>
+        <v>43876.56944444445</v>
       </c>
       <c r="B228" s="1" t="n">
-        <v>43855.56944444445</v>
+        <v>43876.56944444445</v>
       </c>
       <c r="C228" t="n">
         <v>55</v>
@@ -8363,10 +8363,10 @@
     </row>
     <row r="229">
       <c r="A229" s="1" t="n">
-        <v>43855.57638888889</v>
+        <v>43876.57638888889</v>
       </c>
       <c r="B229" s="1" t="n">
-        <v>43855.57638888889</v>
+        <v>43876.57638888889</v>
       </c>
       <c r="C229" t="n">
         <v>55</v>
@@ -8398,10 +8398,10 @@
     </row>
     <row r="230">
       <c r="A230" s="1" t="n">
-        <v>43855.58333333334</v>
+        <v>43876.58333333334</v>
       </c>
       <c r="B230" s="1" t="n">
-        <v>43855.58333333334</v>
+        <v>43876.58333333334</v>
       </c>
       <c r="C230" t="n">
         <v>55</v>
@@ -8433,10 +8433,10 @@
     </row>
     <row r="231">
       <c r="A231" s="1" t="n">
-        <v>43855.59027777778</v>
+        <v>43876.59027777778</v>
       </c>
       <c r="B231" s="1" t="n">
-        <v>43855.59027777778</v>
+        <v>43876.59027777778</v>
       </c>
       <c r="C231" t="n">
         <v>55</v>
@@ -8468,10 +8468,10 @@
     </row>
     <row r="232">
       <c r="A232" s="1" t="n">
-        <v>43855.59722222222</v>
+        <v>43876.59722222222</v>
       </c>
       <c r="B232" s="1" t="n">
-        <v>43855.59722222222</v>
+        <v>43876.59722222222</v>
       </c>
       <c r="C232" t="n">
         <v>55</v>
@@ -8503,10 +8503,10 @@
     </row>
     <row r="233">
       <c r="A233" s="1" t="n">
-        <v>43855.60416666666</v>
+        <v>43876.60416666666</v>
       </c>
       <c r="B233" s="1" t="n">
-        <v>43855.60416666666</v>
+        <v>43876.60416666666</v>
       </c>
       <c r="C233" t="n">
         <v>55</v>
@@ -8538,10 +8538,10 @@
     </row>
     <row r="234">
       <c r="A234" s="1" t="n">
-        <v>43855.61111111111</v>
+        <v>43876.61111111111</v>
       </c>
       <c r="B234" s="1" t="n">
-        <v>43855.61111111111</v>
+        <v>43876.61111111111</v>
       </c>
       <c r="C234" t="n">
         <v>55</v>
@@ -8573,10 +8573,10 @@
     </row>
     <row r="235">
       <c r="A235" s="1" t="n">
-        <v>43855.61805555555</v>
+        <v>43876.61805555555</v>
       </c>
       <c r="B235" s="1" t="n">
-        <v>43855.61805555555</v>
+        <v>43876.61805555555</v>
       </c>
       <c r="C235" t="n">
         <v>55</v>
@@ -8608,10 +8608,10 @@
     </row>
     <row r="236">
       <c r="A236" s="1" t="n">
-        <v>43855.625</v>
+        <v>43876.625</v>
       </c>
       <c r="B236" s="1" t="n">
-        <v>43855.625</v>
+        <v>43876.625</v>
       </c>
       <c r="C236" t="n">
         <v>55</v>
@@ -8643,10 +8643,10 @@
     </row>
     <row r="237">
       <c r="A237" s="1" t="n">
-        <v>43855.63194444445</v>
+        <v>43876.63194444445</v>
       </c>
       <c r="B237" s="1" t="n">
-        <v>43855.63194444445</v>
+        <v>43876.63194444445</v>
       </c>
       <c r="C237" t="n">
         <v>55</v>
@@ -8678,10 +8678,10 @@
     </row>
     <row r="238">
       <c r="A238" s="1" t="n">
-        <v>43855.63888888889</v>
+        <v>43876.63888888889</v>
       </c>
       <c r="B238" s="1" t="n">
-        <v>43855.63888888889</v>
+        <v>43876.63888888889</v>
       </c>
       <c r="C238" t="n">
         <v>55</v>
@@ -8713,10 +8713,10 @@
     </row>
     <row r="239">
       <c r="A239" s="1" t="n">
-        <v>43855.64583333334</v>
+        <v>43876.64583333334</v>
       </c>
       <c r="B239" s="1" t="n">
-        <v>43855.64583333334</v>
+        <v>43876.64583333334</v>
       </c>
       <c r="C239" t="n">
         <v>55</v>
@@ -8748,10 +8748,10 @@
     </row>
     <row r="240">
       <c r="A240" s="1" t="n">
-        <v>43855.65277777778</v>
+        <v>43876.65277777778</v>
       </c>
       <c r="B240" s="1" t="n">
-        <v>43855.65277777778</v>
+        <v>43876.65277777778</v>
       </c>
       <c r="C240" t="n">
         <v>55</v>
@@ -8783,10 +8783,10 @@
     </row>
     <row r="241">
       <c r="A241" s="1" t="n">
-        <v>43855.65972222222</v>
+        <v>43876.65972222222</v>
       </c>
       <c r="B241" s="1" t="n">
-        <v>43855.65972222222</v>
+        <v>43876.65972222222</v>
       </c>
       <c r="C241" t="n">
         <v>55</v>
@@ -8818,10 +8818,10 @@
     </row>
     <row r="242">
       <c r="A242" s="1" t="n">
-        <v>43855.66666666666</v>
+        <v>43876.66666666666</v>
       </c>
       <c r="B242" s="1" t="n">
-        <v>43855.66666666666</v>
+        <v>43876.66666666666</v>
       </c>
       <c r="C242" t="n">
         <v>55</v>
@@ -8853,10 +8853,10 @@
     </row>
     <row r="243">
       <c r="A243" s="1" t="n">
-        <v>43855.67361111111</v>
+        <v>43876.67361111111</v>
       </c>
       <c r="B243" s="1" t="n">
-        <v>43855.67361111111</v>
+        <v>43876.67361111111</v>
       </c>
       <c r="C243" t="n">
         <v>55</v>
@@ -8888,10 +8888,10 @@
     </row>
     <row r="244">
       <c r="A244" s="1" t="n">
-        <v>43855.68055555555</v>
+        <v>43876.68055555555</v>
       </c>
       <c r="B244" s="1" t="n">
-        <v>43855.68055555555</v>
+        <v>43876.68055555555</v>
       </c>
       <c r="C244" t="n">
         <v>55</v>
@@ -8923,10 +8923,10 @@
     </row>
     <row r="245">
       <c r="A245" s="1" t="n">
-        <v>43855.6875</v>
+        <v>43876.6875</v>
       </c>
       <c r="B245" s="1" t="n">
-        <v>43855.6875</v>
+        <v>43876.6875</v>
       </c>
       <c r="C245" t="n">
         <v>55</v>
@@ -8958,10 +8958,10 @@
     </row>
     <row r="246">
       <c r="A246" s="1" t="n">
-        <v>43855.69444444445</v>
+        <v>43876.69444444445</v>
       </c>
       <c r="B246" s="1" t="n">
-        <v>43855.69444444445</v>
+        <v>43876.69444444445</v>
       </c>
       <c r="C246" t="n">
         <v>55</v>
@@ -8993,10 +8993,10 @@
     </row>
     <row r="247">
       <c r="A247" s="1" t="n">
-        <v>43855.70138888889</v>
+        <v>43876.70138888889</v>
       </c>
       <c r="B247" s="1" t="n">
-        <v>43855.70138888889</v>
+        <v>43876.70138888889</v>
       </c>
       <c r="C247" t="n">
         <v>55</v>
@@ -9028,10 +9028,10 @@
     </row>
     <row r="248">
       <c r="A248" s="1" t="n">
-        <v>43855.70833333334</v>
+        <v>43876.70833333334</v>
       </c>
       <c r="B248" s="1" t="n">
-        <v>43855.70833333334</v>
+        <v>43876.70833333334</v>
       </c>
       <c r="C248" t="n">
         <v>55</v>
@@ -9063,10 +9063,10 @@
     </row>
     <row r="249">
       <c r="A249" s="1" t="n">
-        <v>43855.71527777778</v>
+        <v>43876.71527777778</v>
       </c>
       <c r="B249" s="1" t="n">
-        <v>43855.71527777778</v>
+        <v>43876.71527777778</v>
       </c>
       <c r="C249" t="n">
         <v>55</v>
@@ -9098,10 +9098,10 @@
     </row>
     <row r="250">
       <c r="A250" s="1" t="n">
-        <v>43855.72222222222</v>
+        <v>43876.72222222222</v>
       </c>
       <c r="B250" s="1" t="n">
-        <v>43855.72222222222</v>
+        <v>43876.72222222222</v>
       </c>
       <c r="C250" t="n">
         <v>55</v>
@@ -9133,10 +9133,10 @@
     </row>
     <row r="251">
       <c r="A251" s="1" t="n">
-        <v>43855.72916666666</v>
+        <v>43876.72916666666</v>
       </c>
       <c r="B251" s="1" t="n">
-        <v>43855.72916666666</v>
+        <v>43876.72916666666</v>
       </c>
       <c r="C251" t="n">
         <v>55</v>
@@ -9168,10 +9168,10 @@
     </row>
     <row r="252">
       <c r="A252" s="1" t="n">
-        <v>43855.73611111111</v>
+        <v>43876.73611111111</v>
       </c>
       <c r="B252" s="1" t="n">
-        <v>43855.73611111111</v>
+        <v>43876.73611111111</v>
       </c>
       <c r="C252" t="n">
         <v>55</v>
@@ -9203,10 +9203,10 @@
     </row>
     <row r="253">
       <c r="A253" s="1" t="n">
-        <v>43855.74305555555</v>
+        <v>43876.74305555555</v>
       </c>
       <c r="B253" s="1" t="n">
-        <v>43855.74305555555</v>
+        <v>43876.74305555555</v>
       </c>
       <c r="C253" t="n">
         <v>55</v>
@@ -9238,10 +9238,10 @@
     </row>
     <row r="254">
       <c r="A254" s="1" t="n">
-        <v>43855.75</v>
+        <v>43876.75</v>
       </c>
       <c r="B254" s="1" t="n">
-        <v>43855.75</v>
+        <v>43876.75</v>
       </c>
       <c r="C254" t="n">
         <v>55</v>
@@ -9273,10 +9273,10 @@
     </row>
     <row r="255">
       <c r="A255" s="1" t="n">
-        <v>43855.75694444445</v>
+        <v>43876.75694444445</v>
       </c>
       <c r="B255" s="1" t="n">
-        <v>43855.75694444445</v>
+        <v>43876.75694444445</v>
       </c>
       <c r="C255" t="n">
         <v>55</v>
@@ -9308,10 +9308,10 @@
     </row>
     <row r="256">
       <c r="A256" s="1" t="n">
-        <v>43855.76388888889</v>
+        <v>43876.76388888889</v>
       </c>
       <c r="B256" s="1" t="n">
-        <v>43855.76388888889</v>
+        <v>43876.76388888889</v>
       </c>
       <c r="C256" t="n">
         <v>55</v>
@@ -9343,10 +9343,10 @@
     </row>
     <row r="257">
       <c r="A257" s="1" t="n">
-        <v>43855.77083333334</v>
+        <v>43876.77083333334</v>
       </c>
       <c r="B257" s="1" t="n">
-        <v>43855.77083333334</v>
+        <v>43876.77083333334</v>
       </c>
       <c r="C257" t="n">
         <v>55</v>
@@ -9378,10 +9378,10 @@
     </row>
     <row r="258">
       <c r="A258" s="1" t="n">
-        <v>43855.77777777778</v>
+        <v>43876.77777777778</v>
       </c>
       <c r="B258" s="1" t="n">
-        <v>43855.77777777778</v>
+        <v>43876.77777777778</v>
       </c>
       <c r="C258" t="n">
         <v>55</v>
@@ -9413,10 +9413,10 @@
     </row>
     <row r="259">
       <c r="A259" s="1" t="n">
-        <v>43855.78472222222</v>
+        <v>43876.78472222222</v>
       </c>
       <c r="B259" s="1" t="n">
-        <v>43855.78472222222</v>
+        <v>43876.78472222222</v>
       </c>
       <c r="C259" t="n">
         <v>55</v>
@@ -9448,10 +9448,10 @@
     </row>
     <row r="260">
       <c r="A260" s="1" t="n">
-        <v>43855.79166666666</v>
+        <v>43876.79166666666</v>
       </c>
       <c r="B260" s="1" t="n">
-        <v>43855.79166666666</v>
+        <v>43876.79166666666</v>
       </c>
       <c r="C260" t="n">
         <v>55</v>
@@ -9483,10 +9483,10 @@
     </row>
     <row r="261">
       <c r="A261" s="1" t="n">
-        <v>43855.79861111111</v>
+        <v>43876.79861111111</v>
       </c>
       <c r="B261" s="1" t="n">
-        <v>43855.79861111111</v>
+        <v>43876.79861111111</v>
       </c>
       <c r="C261" t="n">
         <v>55</v>
@@ -9518,10 +9518,10 @@
     </row>
     <row r="262">
       <c r="A262" s="1" t="n">
-        <v>43855.80555555555</v>
+        <v>43876.80555555555</v>
       </c>
       <c r="B262" s="1" t="n">
-        <v>43855.80555555555</v>
+        <v>43876.80555555555</v>
       </c>
       <c r="C262" t="n">
         <v>55</v>
@@ -9553,10 +9553,10 @@
     </row>
     <row r="263">
       <c r="A263" s="1" t="n">
-        <v>43855.8125</v>
+        <v>43876.8125</v>
       </c>
       <c r="B263" s="1" t="n">
-        <v>43855.8125</v>
+        <v>43876.8125</v>
       </c>
       <c r="C263" t="n">
         <v>55</v>
@@ -9588,10 +9588,10 @@
     </row>
     <row r="264">
       <c r="A264" s="1" t="n">
-        <v>43855.81944444445</v>
+        <v>43876.81944444445</v>
       </c>
       <c r="B264" s="1" t="n">
-        <v>43855.81944444445</v>
+        <v>43876.81944444445</v>
       </c>
       <c r="C264" t="n">
         <v>55</v>
@@ -9623,10 +9623,10 @@
     </row>
     <row r="265">
       <c r="A265" s="1" t="n">
-        <v>43855.82638888889</v>
+        <v>43876.82638888889</v>
       </c>
       <c r="B265" s="1" t="n">
-        <v>43855.82638888889</v>
+        <v>43876.82638888889</v>
       </c>
       <c r="C265" t="n">
         <v>55</v>
@@ -9658,10 +9658,10 @@
     </row>
     <row r="266">
       <c r="A266" s="1" t="n">
-        <v>43855.83333333334</v>
+        <v>43876.83333333334</v>
       </c>
       <c r="B266" s="1" t="n">
-        <v>43855.83333333334</v>
+        <v>43876.83333333334</v>
       </c>
       <c r="C266" t="n">
         <v>55</v>
@@ -9693,10 +9693,10 @@
     </row>
     <row r="267">
       <c r="A267" s="1" t="n">
-        <v>43855.84027777778</v>
+        <v>43876.84027777778</v>
       </c>
       <c r="B267" s="1" t="n">
-        <v>43855.84027777778</v>
+        <v>43876.84027777778</v>
       </c>
       <c r="C267" t="n">
         <v>55</v>
@@ -9728,10 +9728,10 @@
     </row>
     <row r="268">
       <c r="A268" s="1" t="n">
-        <v>43855.84722222222</v>
+        <v>43876.84722222222</v>
       </c>
       <c r="B268" s="1" t="n">
-        <v>43855.84722222222</v>
+        <v>43876.84722222222</v>
       </c>
       <c r="C268" t="n">
         <v>55</v>
@@ -9763,10 +9763,10 @@
     </row>
     <row r="269">
       <c r="A269" s="1" t="n">
-        <v>43855.85416666666</v>
+        <v>43876.85416666666</v>
       </c>
       <c r="B269" s="1" t="n">
-        <v>43855.85416666666</v>
+        <v>43876.85416666666</v>
       </c>
       <c r="C269" t="n">
         <v>55</v>
@@ -9798,10 +9798,10 @@
     </row>
     <row r="270">
       <c r="A270" s="1" t="n">
-        <v>43855.86111111111</v>
+        <v>43876.86111111111</v>
       </c>
       <c r="B270" s="1" t="n">
-        <v>43855.86111111111</v>
+        <v>43876.86111111111</v>
       </c>
       <c r="C270" t="n">
         <v>55</v>
@@ -9833,10 +9833,10 @@
     </row>
     <row r="271">
       <c r="A271" s="1" t="n">
-        <v>43855.86805555555</v>
+        <v>43876.86805555555</v>
       </c>
       <c r="B271" s="1" t="n">
-        <v>43855.86805555555</v>
+        <v>43876.86805555555</v>
       </c>
       <c r="C271" t="n">
         <v>55</v>
@@ -9868,10 +9868,10 @@
     </row>
     <row r="272">
       <c r="A272" s="1" t="n">
-        <v>43855.875</v>
+        <v>43876.875</v>
       </c>
       <c r="B272" s="1" t="n">
-        <v>43855.875</v>
+        <v>43876.875</v>
       </c>
       <c r="C272" t="n">
         <v>55</v>
@@ -9903,10 +9903,10 @@
     </row>
     <row r="273">
       <c r="A273" s="1" t="n">
-        <v>43855.88194444445</v>
+        <v>43876.88194444445</v>
       </c>
       <c r="B273" s="1" t="n">
-        <v>43855.88194444445</v>
+        <v>43876.88194444445</v>
       </c>
       <c r="C273" t="n">
         <v>55</v>
@@ -9938,10 +9938,10 @@
     </row>
     <row r="274">
       <c r="A274" s="1" t="n">
-        <v>43855.88888888889</v>
+        <v>43876.88888888889</v>
       </c>
       <c r="B274" s="1" t="n">
-        <v>43855.88888888889</v>
+        <v>43876.88888888889</v>
       </c>
       <c r="C274" t="n">
         <v>55</v>
@@ -9973,10 +9973,10 @@
     </row>
     <row r="275">
       <c r="A275" s="1" t="n">
-        <v>43855.89583333334</v>
+        <v>43876.89583333334</v>
       </c>
       <c r="B275" s="1" t="n">
-        <v>43855.89583333334</v>
+        <v>43876.89583333334</v>
       </c>
       <c r="C275" t="n">
         <v>55</v>
@@ -10008,10 +10008,10 @@
     </row>
     <row r="276">
       <c r="A276" s="1" t="n">
-        <v>43855.90277777778</v>
+        <v>43876.90277777778</v>
       </c>
       <c r="B276" s="1" t="n">
-        <v>43855.90277777778</v>
+        <v>43876.90277777778</v>
       </c>
       <c r="C276" t="n">
         <v>55</v>
@@ -10043,10 +10043,10 @@
     </row>
     <row r="277">
       <c r="A277" s="1" t="n">
-        <v>43855.90972222222</v>
+        <v>43876.90972222222</v>
       </c>
       <c r="B277" s="1" t="n">
-        <v>43855.90972222222</v>
+        <v>43876.90972222222</v>
       </c>
       <c r="C277" t="n">
         <v>55</v>
@@ -10078,10 +10078,10 @@
     </row>
     <row r="278">
       <c r="A278" s="1" t="n">
-        <v>43855.91666666666</v>
+        <v>43876.91666666666</v>
       </c>
       <c r="B278" s="1" t="n">
-        <v>43855.91666666666</v>
+        <v>43876.91666666666</v>
       </c>
       <c r="C278" t="n">
         <v>55</v>
@@ -10113,10 +10113,10 @@
     </row>
     <row r="279">
       <c r="A279" s="1" t="n">
-        <v>43855.92361111111</v>
+        <v>43876.92361111111</v>
       </c>
       <c r="B279" s="1" t="n">
-        <v>43855.92361111111</v>
+        <v>43876.92361111111</v>
       </c>
       <c r="C279" t="n">
         <v>55</v>
@@ -10148,10 +10148,10 @@
     </row>
     <row r="280">
       <c r="A280" s="1" t="n">
-        <v>43855.93055555555</v>
+        <v>43876.93055555555</v>
       </c>
       <c r="B280" s="1" t="n">
-        <v>43855.93055555555</v>
+        <v>43876.93055555555</v>
       </c>
       <c r="C280" t="n">
         <v>55</v>
@@ -10183,10 +10183,10 @@
     </row>
     <row r="281">
       <c r="A281" s="1" t="n">
-        <v>43855.9375</v>
+        <v>43876.9375</v>
       </c>
       <c r="B281" s="1" t="n">
-        <v>43855.9375</v>
+        <v>43876.9375</v>
       </c>
       <c r="C281" t="n">
         <v>55</v>
@@ -10218,10 +10218,10 @@
     </row>
     <row r="282">
       <c r="A282" s="1" t="n">
-        <v>43855.94444444445</v>
+        <v>43876.94444444445</v>
       </c>
       <c r="B282" s="1" t="n">
-        <v>43855.94444444445</v>
+        <v>43876.94444444445</v>
       </c>
       <c r="C282" t="n">
         <v>55</v>
@@ -10253,10 +10253,10 @@
     </row>
     <row r="283">
       <c r="A283" s="1" t="n">
-        <v>43855.95138888889</v>
+        <v>43876.95138888889</v>
       </c>
       <c r="B283" s="1" t="n">
-        <v>43855.95138888889</v>
+        <v>43876.95138888889</v>
       </c>
       <c r="C283" t="n">
         <v>55</v>
@@ -10288,10 +10288,10 @@
     </row>
     <row r="284">
       <c r="A284" s="1" t="n">
-        <v>43855.95833333334</v>
+        <v>43876.95833333334</v>
       </c>
       <c r="B284" s="1" t="n">
-        <v>43855.95833333334</v>
+        <v>43876.95833333334</v>
       </c>
       <c r="C284" t="n">
         <v>55</v>
@@ -10323,10 +10323,10 @@
     </row>
     <row r="285">
       <c r="A285" s="1" t="n">
-        <v>43855.96527777778</v>
+        <v>43876.96527777778</v>
       </c>
       <c r="B285" s="1" t="n">
-        <v>43855.96527777778</v>
+        <v>43876.96527777778</v>
       </c>
       <c r="C285" t="n">
         <v>55</v>
@@ -10358,10 +10358,10 @@
     </row>
     <row r="286">
       <c r="A286" s="1" t="n">
-        <v>43855.97222222222</v>
+        <v>43876.97222222222</v>
       </c>
       <c r="B286" s="1" t="n">
-        <v>43855.97222222222</v>
+        <v>43876.97222222222</v>
       </c>
       <c r="C286" t="n">
         <v>55</v>
@@ -10393,10 +10393,10 @@
     </row>
     <row r="287">
       <c r="A287" s="1" t="n">
-        <v>43855.97916666666</v>
+        <v>43876.97916666666</v>
       </c>
       <c r="B287" s="1" t="n">
-        <v>43855.97916666666</v>
+        <v>43876.97916666666</v>
       </c>
       <c r="C287" t="n">
         <v>55</v>
@@ -10428,10 +10428,10 @@
     </row>
     <row r="288">
       <c r="A288" s="1" t="n">
-        <v>43855.98611111111</v>
+        <v>43876.98611111111</v>
       </c>
       <c r="B288" s="1" t="n">
-        <v>43855.98611111111</v>
+        <v>43876.98611111111</v>
       </c>
       <c r="C288" t="n">
         <v>55</v>
@@ -10463,10 +10463,10 @@
     </row>
     <row r="289">
       <c r="A289" s="1" t="n">
-        <v>43855.99305555555</v>
+        <v>43876.99305555555</v>
       </c>
       <c r="B289" s="1" t="n">
-        <v>43855.99305555555</v>
+        <v>43876.99305555555</v>
       </c>
       <c r="C289" t="n">
         <v>55</v>

</xml_diff>